<commit_message>
Reorganize feature files and step definitions with improved naming and test data structure
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ApacheExcel.xlsx
+++ b/src/test/java/apachePOI/resource/ApacheExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13980" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,10 @@
     <t>End</t>
   </si>
   <si>
-    <t>Turkish012</t>
-  </si>
-  <si>
-    <t>trksh12</t>
+    <t>Turkish - TR</t>
+  </si>
+  <si>
+    <t>TR-CTZ</t>
   </si>
   <si>
     <t>one</t>
@@ -66,10 +66,10 @@
     <t>four</t>
   </si>
   <si>
-    <t>Kurdish012</t>
-  </si>
-  <si>
-    <t>krdsh12</t>
+    <t>Kurdish - KU</t>
+  </si>
+  <si>
+    <t>KU-CTZ</t>
   </si>
   <si>
     <t>two</t>
@@ -78,40 +78,40 @@
     <t>five</t>
   </si>
   <si>
-    <t>German012</t>
-  </si>
-  <si>
-    <t>grmn12</t>
-  </si>
-  <si>
-    <t>English012</t>
-  </si>
-  <si>
-    <t>eng12</t>
-  </si>
-  <si>
-    <t>Norwegian012</t>
-  </si>
-  <si>
-    <t>nrwgn12</t>
-  </si>
-  <si>
-    <t>Italian012</t>
-  </si>
-  <si>
-    <t>itln12</t>
-  </si>
-  <si>
-    <t>Spanish012</t>
-  </si>
-  <si>
-    <t>spnsh12</t>
-  </si>
-  <si>
-    <t>American012</t>
-  </si>
-  <si>
-    <t>amrcn12</t>
+    <t>German - DE</t>
+  </si>
+  <si>
+    <t>DE-CTZ</t>
+  </si>
+  <si>
+    <t>English - EN</t>
+  </si>
+  <si>
+    <t>EN-CTZ</t>
+  </si>
+  <si>
+    <t>Norwegian - NO</t>
+  </si>
+  <si>
+    <t>NO-CTZ</t>
+  </si>
+  <si>
+    <t>Italian - IT</t>
+  </si>
+  <si>
+    <t>IT-CTZ</t>
+  </si>
+  <si>
+    <t>Spanish - ES</t>
+  </si>
+  <si>
+    <t>ES-CTZ</t>
+  </si>
+  <si>
+    <t>American - US</t>
+  </si>
+  <si>
+    <t>US-CTZ</t>
   </si>
 </sst>
 </file>
@@ -725,8 +725,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1063,7 +1066,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1071,7 +1074,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -1085,7 +1088,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1093,7 +1096,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>8</v>
       </c>
     </row>
@@ -1139,7 +1142,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="5"/>
@@ -1148,7 +1151,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
@@ -1168,7 +1171,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
@@ -1188,7 +1191,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
@@ -1208,7 +1211,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
@@ -1228,7 +1231,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
@@ -1240,7 +1243,7 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
@@ -1248,7 +1251,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
@@ -1268,7 +1271,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
@@ -1288,7 +1291,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
@@ -1300,7 +1303,7 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">

</xml_diff>